<commit_message>
Fixing bug and data value
</commit_message>
<xml_diff>
--- a/MortalityData/HIVStandardisedMortalityRateOriginalValuesFromStudy.xlsx
+++ b/MortalityData/HIVStandardisedMortalityRateOriginalValuesFromStudy.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="480" yWindow="45" windowWidth="21915" windowHeight="12780"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="11">
   <si>
     <t>Min age</t>
   </si>
@@ -47,12 +47,15 @@
   <si>
     <t>*recalculated and confirmed</t>
   </si>
+  <si>
+    <t>* 45-54 in 1990 paper quoted 41.13, using 24.94</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -98,6 +101,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -176,6 +184,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -210,6 +219,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -385,16 +395,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+      <selection activeCell="O17" sqref="O17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:15">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -405,7 +415,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:15">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C2" t="s">
         <v>3</v>
       </c>
@@ -443,7 +453,7 @@
         <v>1997</v>
       </c>
     </row>
-    <row r="3" spans="1:15">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -487,7 +497,7 @@
         <v>3000</v>
       </c>
     </row>
-    <row r="4" spans="1:15">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>0</v>
       </c>
@@ -522,7 +532,7 @@
         <v>6.01</v>
       </c>
     </row>
-    <row r="5" spans="1:15">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>25</v>
       </c>
@@ -563,7 +573,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:15">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>35</v>
       </c>
@@ -598,7 +608,7 @@
         <v>2.38</v>
       </c>
     </row>
-    <row r="7" spans="1:15">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>45</v>
       </c>
@@ -633,7 +643,7 @@
         <v>1.76</v>
       </c>
     </row>
-    <row r="8" spans="1:15">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>55</v>
       </c>
@@ -668,7 +678,7 @@
         <v>1.24</v>
       </c>
     </row>
-    <row r="9" spans="1:15">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>65</v>
       </c>
@@ -703,7 +713,7 @@
         <v>0.84</v>
       </c>
     </row>
-    <row r="11" spans="1:15">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>5</v>
       </c>
@@ -714,7 +724,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:15">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C12" t="s">
         <v>3</v>
       </c>
@@ -752,7 +762,7 @@
         <v>1997</v>
       </c>
     </row>
-    <row r="13" spans="1:15">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>0</v>
       </c>
@@ -796,7 +806,7 @@
         <v>3000</v>
       </c>
     </row>
-    <row r="14" spans="1:15">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>0</v>
       </c>
@@ -831,7 +841,7 @@
         <v>36.020000000000003</v>
       </c>
     </row>
-    <row r="15" spans="1:15">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>25</v>
       </c>
@@ -866,7 +876,7 @@
         <v>16.190000000000001</v>
       </c>
     </row>
-    <row r="16" spans="1:15">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>35</v>
       </c>
@@ -904,7 +914,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="17" spans="1:15">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>45</v>
       </c>
@@ -914,8 +924,8 @@
       <c r="D17">
         <v>95.64</v>
       </c>
-      <c r="E17">
-        <v>41.13</v>
+      <c r="E17" s="1">
+        <v>24.94</v>
       </c>
       <c r="F17">
         <v>4.25</v>
@@ -938,8 +948,11 @@
       <c r="N17">
         <v>4.4720000000000004</v>
       </c>
-    </row>
-    <row r="18" spans="1:15">
+      <c r="O17" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>55</v>
       </c>
@@ -974,7 +987,7 @@
         <v>2.84</v>
       </c>
     </row>
-    <row r="19" spans="1:15">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>65</v>
       </c>
@@ -1019,24 +1032,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>